<commit_message>
Improved use of data New data sets created for exposure time
</commit_message>
<xml_diff>
--- a/Dataset hond-katFV20210128.xlsx
+++ b/Dataset hond-katFV20210128.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/f_c_velkers_uu_nl/Documents/Nertsen-Covid/Paola en Wendy/Kattenproject/Bronnen paper Anna 210125/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Surfdrive\Projecten\Covid\CatsAndMink\mink-cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19C72903-0002-4330-91F3-C43D5A9C19E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44450DDA-3D42-4916-B37E-DF48EC64F470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NC_KAT 11-Aug-2020" sheetId="1" r:id="rId1"/>
@@ -503,8 +503,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/mm/yy;@"/>
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -638,7 +639,6 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -701,6 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -1050,7 +1051,7 @@
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="4" max="4" width="11" style="25" customWidth="1"/>
     <col min="5" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
@@ -1068,7 +1069,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1127,7 +1128,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="25">
         <v>43958</v>
       </c>
       <c r="E2">
@@ -1180,7 +1181,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="25">
         <v>43958</v>
       </c>
       <c r="E3">
@@ -1233,7 +1234,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="25">
         <v>43958</v>
       </c>
       <c r="E4">
@@ -1286,7 +1287,7 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="25">
         <v>43958</v>
       </c>
       <c r="E5">
@@ -1336,7 +1337,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="25">
         <v>43958</v>
       </c>
       <c r="E6">
@@ -1389,7 +1390,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="25">
         <v>43958</v>
       </c>
       <c r="E7">
@@ -1442,7 +1443,7 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="25">
         <v>43958</v>
       </c>
       <c r="E8">
@@ -1495,7 +1496,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="25">
         <v>43958</v>
       </c>
       <c r="E9">
@@ -1548,7 +1549,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="25">
         <v>43958</v>
       </c>
       <c r="E10">
@@ -1601,7 +1602,7 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="25">
         <v>43958</v>
       </c>
       <c r="E11">
@@ -1648,7 +1649,7 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="25">
         <v>43958</v>
       </c>
       <c r="E12">
@@ -1695,7 +1696,7 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="25">
         <v>43958</v>
       </c>
       <c r="E13">
@@ -1742,7 +1743,7 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="25">
         <v>43958</v>
       </c>
       <c r="E14">
@@ -1795,7 +1796,7 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="25">
         <v>43958</v>
       </c>
       <c r="E15">
@@ -1848,7 +1849,7 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="25">
         <v>43968</v>
       </c>
       <c r="E16">
@@ -1901,7 +1902,7 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="25">
         <v>43968</v>
       </c>
       <c r="E17">
@@ -1954,7 +1955,7 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="25">
         <v>43968</v>
       </c>
       <c r="E18">
@@ -2007,7 +2008,7 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="25">
         <v>43968</v>
       </c>
       <c r="E19">
@@ -2063,7 +2064,7 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="25">
         <v>43968</v>
       </c>
       <c r="E20">
@@ -2116,7 +2117,7 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="25">
         <v>43968</v>
       </c>
       <c r="E21">
@@ -2169,7 +2170,7 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="25">
         <v>43968</v>
       </c>
       <c r="E22">
@@ -2222,7 +2223,7 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="25">
         <v>43968</v>
       </c>
       <c r="E23">
@@ -2275,7 +2276,7 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="25">
         <v>43968</v>
       </c>
       <c r="E24">
@@ -2328,7 +2329,7 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="25">
         <v>43968</v>
       </c>
       <c r="E25">
@@ -2375,7 +2376,7 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="25">
         <v>43968</v>
       </c>
       <c r="E26">
@@ -2428,7 +2429,7 @@
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="25">
         <v>43968</v>
       </c>
       <c r="E27">
@@ -2481,7 +2482,7 @@
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="25">
         <v>43968</v>
       </c>
       <c r="E28">
@@ -2534,7 +2535,7 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="25">
         <v>43968</v>
       </c>
       <c r="E29">
@@ -2587,7 +2588,7 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="25">
         <v>43968</v>
       </c>
       <c r="E30">
@@ -2640,7 +2641,7 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="25">
         <v>43968</v>
       </c>
       <c r="E31">
@@ -2687,7 +2688,7 @@
       <c r="C32">
         <v>3</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="25">
         <v>43973</v>
       </c>
       <c r="E32">
@@ -2740,7 +2741,7 @@
       <c r="C33">
         <v>3</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="25">
         <v>43973</v>
       </c>
       <c r="E33">
@@ -2793,7 +2794,7 @@
       <c r="C34">
         <v>3</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="25">
         <v>43973</v>
       </c>
       <c r="E34">
@@ -2846,7 +2847,7 @@
       <c r="C35">
         <v>3</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="25">
         <v>43973</v>
       </c>
       <c r="E35">
@@ -2899,7 +2900,7 @@
       <c r="C36">
         <v>3</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="25">
         <v>43973</v>
       </c>
       <c r="E36">
@@ -2952,7 +2953,7 @@
       <c r="C37">
         <v>3</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="25">
         <v>43973</v>
       </c>
       <c r="E37">
@@ -3002,7 +3003,7 @@
       <c r="C38">
         <v>3</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="25">
         <v>43973</v>
       </c>
       <c r="E38">
@@ -3052,7 +3053,7 @@
       <c r="C39">
         <v>3</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="25">
         <v>43973</v>
       </c>
       <c r="E39">
@@ -3102,7 +3103,7 @@
       <c r="C40">
         <v>1</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="25">
         <v>43973</v>
       </c>
       <c r="E40">
@@ -3149,7 +3150,7 @@
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="25">
         <v>43973</v>
       </c>
       <c r="E41">
@@ -3196,7 +3197,7 @@
       <c r="C42">
         <v>1</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="25">
         <v>43973</v>
       </c>
       <c r="E42">
@@ -3243,7 +3244,7 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="25">
         <v>43973</v>
       </c>
       <c r="E43">
@@ -3290,7 +3291,7 @@
       <c r="C44">
         <v>1</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="25">
         <v>43973</v>
       </c>
       <c r="E44">
@@ -3337,7 +3338,7 @@
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="25">
         <v>43973</v>
       </c>
       <c r="E45">
@@ -3384,7 +3385,7 @@
       <c r="C46">
         <v>1</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="25">
         <v>43973</v>
       </c>
       <c r="E46">
@@ -3431,7 +3432,7 @@
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="25">
         <v>43973</v>
       </c>
       <c r="E47">
@@ -3478,7 +3479,7 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="25">
         <v>43973</v>
       </c>
       <c r="E48">
@@ -3525,7 +3526,7 @@
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="25">
         <v>43973</v>
       </c>
       <c r="E49">
@@ -3572,7 +3573,7 @@
       <c r="C50">
         <v>4</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="25">
         <v>43981</v>
       </c>
       <c r="E50">
@@ -3625,7 +3626,7 @@
       <c r="C51">
         <v>4</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="25">
         <v>43981</v>
       </c>
       <c r="E51">
@@ -3678,7 +3679,7 @@
       <c r="C52">
         <v>4</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="25">
         <v>43981</v>
       </c>
       <c r="E52">
@@ -3731,7 +3732,7 @@
       <c r="C53">
         <v>4</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="25">
         <v>43981</v>
       </c>
       <c r="E53">
@@ -3784,7 +3785,7 @@
       <c r="C54">
         <v>4</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="25">
         <v>43981</v>
       </c>
       <c r="E54">
@@ -3840,7 +3841,7 @@
       <c r="C55">
         <v>4</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="25">
         <v>43981</v>
       </c>
       <c r="E55">
@@ -3893,7 +3894,7 @@
       <c r="C56">
         <v>4</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="25">
         <v>43981</v>
       </c>
       <c r="E56">
@@ -3946,7 +3947,7 @@
       <c r="C57">
         <v>4</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="25">
         <v>43981</v>
       </c>
       <c r="E57">
@@ -3996,7 +3997,7 @@
       <c r="C58">
         <v>4</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="25">
         <v>43981</v>
       </c>
       <c r="E58">
@@ -4046,7 +4047,7 @@
       <c r="C59">
         <v>4</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="25">
         <v>43981</v>
       </c>
       <c r="E59">
@@ -4096,7 +4097,7 @@
       <c r="C60">
         <v>4</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="25">
         <v>43981</v>
       </c>
       <c r="E60">
@@ -4149,7 +4150,7 @@
       <c r="C61">
         <v>4</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="25">
         <v>43981</v>
       </c>
       <c r="E61">
@@ -4202,7 +4203,7 @@
       <c r="C62">
         <v>4</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="25">
         <v>43981</v>
       </c>
       <c r="E62">
@@ -4255,7 +4256,7 @@
       <c r="C63">
         <v>4</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="25">
         <v>43981</v>
       </c>
       <c r="E63">
@@ -4302,7 +4303,7 @@
       <c r="C64">
         <v>4</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="25">
         <v>43981</v>
       </c>
       <c r="E64">
@@ -4349,7 +4350,7 @@
       <c r="C65">
         <v>4</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="25">
         <v>43981</v>
       </c>
       <c r="E65">
@@ -4396,7 +4397,7 @@
       <c r="C66">
         <v>4</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="25">
         <v>43981</v>
       </c>
       <c r="E66">
@@ -4443,7 +4444,7 @@
       <c r="C67">
         <v>4</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="25">
         <v>43981</v>
       </c>
       <c r="E67">
@@ -4490,7 +4491,7 @@
       <c r="C68">
         <v>4</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68" s="25">
         <v>43981</v>
       </c>
       <c r="E68">
@@ -4537,7 +4538,7 @@
       <c r="C69">
         <v>7</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="25">
         <v>43994</v>
       </c>
       <c r="E69">
@@ -4570,7 +4571,7 @@
       <c r="N69">
         <v>0</v>
       </c>
-      <c r="O69" s="9">
+      <c r="O69" s="8">
         <v>0</v>
       </c>
       <c r="P69">
@@ -4590,7 +4591,7 @@
       <c r="C70">
         <v>7</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70" s="25">
         <v>43994</v>
       </c>
       <c r="E70">
@@ -4623,7 +4624,7 @@
       <c r="N70">
         <v>0</v>
       </c>
-      <c r="O70" s="9">
+      <c r="O70" s="8">
         <v>0</v>
       </c>
       <c r="P70">
@@ -4643,7 +4644,7 @@
       <c r="C71">
         <v>7</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="25">
         <v>43994</v>
       </c>
       <c r="E71">
@@ -4676,7 +4677,7 @@
       <c r="N71">
         <v>0</v>
       </c>
-      <c r="O71" s="9">
+      <c r="O71" s="8">
         <v>0</v>
       </c>
       <c r="P71">
@@ -4696,7 +4697,7 @@
       <c r="C72">
         <v>7</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72" s="25">
         <v>43994</v>
       </c>
       <c r="E72">
@@ -4729,7 +4730,7 @@
       <c r="N72">
         <v>0</v>
       </c>
-      <c r="O72" s="9">
+      <c r="O72" s="8">
         <v>0</v>
       </c>
       <c r="P72">
@@ -4749,7 +4750,7 @@
       <c r="C73">
         <v>7</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="25">
         <v>43994</v>
       </c>
       <c r="E73">
@@ -4782,7 +4783,7 @@
       <c r="N73">
         <v>0</v>
       </c>
-      <c r="O73" s="9">
+      <c r="O73" s="8">
         <v>0</v>
       </c>
       <c r="P73">
@@ -4802,7 +4803,7 @@
       <c r="C74">
         <v>7</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="25">
         <v>43994</v>
       </c>
       <c r="E74">
@@ -4835,7 +4836,7 @@
       <c r="N74">
         <v>0</v>
       </c>
-      <c r="O74" s="9">
+      <c r="O74" s="8">
         <v>0</v>
       </c>
       <c r="P74">
@@ -4855,7 +4856,7 @@
       <c r="C75">
         <v>7</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="25">
         <v>43994</v>
       </c>
       <c r="E75">
@@ -4902,7 +4903,7 @@
       <c r="C76">
         <v>7</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="25">
         <v>43994</v>
       </c>
       <c r="E76">
@@ -4949,7 +4950,7 @@
       <c r="C77">
         <v>7</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77" s="25">
         <v>43994</v>
       </c>
       <c r="E77">
@@ -4996,7 +4997,7 @@
       <c r="C78">
         <v>7</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="25">
         <v>43994</v>
       </c>
       <c r="E78">
@@ -5043,7 +5044,7 @@
       <c r="C79">
         <v>7</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79" s="25">
         <v>43994</v>
       </c>
       <c r="E79">
@@ -5090,7 +5091,7 @@
       <c r="C80">
         <v>7</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80" s="25">
         <v>43994</v>
       </c>
       <c r="E80">
@@ -5137,7 +5138,7 @@
       <c r="C81">
         <v>7</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="25">
         <v>43994</v>
       </c>
       <c r="E81">
@@ -5184,7 +5185,7 @@
       <c r="C82">
         <v>7</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82" s="25">
         <v>43994</v>
       </c>
       <c r="E82">
@@ -5231,7 +5232,7 @@
       <c r="C83">
         <v>7</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83" s="25">
         <v>43994</v>
       </c>
       <c r="E83">
@@ -5258,7 +5259,7 @@
       <c r="L83">
         <v>0</v>
       </c>
-      <c r="M83" s="7" t="s">
+      <c r="M83" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P83">
@@ -5278,7 +5279,7 @@
       <c r="C84">
         <v>13</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D84" s="25">
         <v>44026</v>
       </c>
       <c r="E84">
@@ -5305,13 +5306,13 @@
       <c r="L84">
         <v>1</v>
       </c>
-      <c r="M84" s="8" t="s">
+      <c r="M84" s="7" t="s">
         <v>106</v>
       </c>
       <c r="N84">
         <v>0</v>
       </c>
-      <c r="O84" s="9">
+      <c r="O84" s="8">
         <v>0</v>
       </c>
       <c r="P84">
@@ -5331,7 +5332,7 @@
       <c r="C85">
         <v>13</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="25">
         <v>44026</v>
       </c>
       <c r="E85">
@@ -5358,13 +5359,13 @@
       <c r="L85">
         <v>1</v>
       </c>
-      <c r="M85" s="8" t="s">
+      <c r="M85" s="7" t="s">
         <v>107</v>
       </c>
       <c r="N85">
         <v>0</v>
       </c>
-      <c r="O85" s="9">
+      <c r="O85" s="8">
         <v>0</v>
       </c>
       <c r="P85">
@@ -5384,7 +5385,7 @@
       <c r="C86">
         <v>13</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="25">
         <v>44026</v>
       </c>
       <c r="E86">
@@ -5411,13 +5412,13 @@
       <c r="L86">
         <v>1</v>
       </c>
-      <c r="M86" s="8" t="s">
+      <c r="M86" s="7" t="s">
         <v>108</v>
       </c>
       <c r="N86">
         <v>0</v>
       </c>
-      <c r="O86" s="9">
+      <c r="O86" s="8">
         <v>0</v>
       </c>
       <c r="P86">
@@ -5437,7 +5438,7 @@
       <c r="C87">
         <v>13</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="25">
         <v>44026</v>
       </c>
       <c r="E87">
@@ -5464,13 +5465,13 @@
       <c r="L87">
         <v>1</v>
       </c>
-      <c r="M87" s="8" t="s">
+      <c r="M87" s="7" t="s">
         <v>109</v>
       </c>
       <c r="N87">
         <v>0</v>
       </c>
-      <c r="O87" s="9">
+      <c r="O87" s="8">
         <v>0</v>
       </c>
       <c r="P87">
@@ -5490,7 +5491,7 @@
       <c r="C88">
         <v>13</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D88" s="25">
         <v>44026</v>
       </c>
       <c r="E88">
@@ -5517,13 +5518,13 @@
       <c r="L88">
         <v>1</v>
       </c>
-      <c r="M88" s="8" t="s">
+      <c r="M88" s="7" t="s">
         <v>110</v>
       </c>
       <c r="N88">
         <v>0</v>
       </c>
-      <c r="O88" s="9">
+      <c r="O88" s="8">
         <v>0</v>
       </c>
       <c r="P88">
@@ -5543,7 +5544,7 @@
       <c r="C89">
         <v>13</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D89" s="25">
         <v>44026</v>
       </c>
       <c r="E89">
@@ -5570,13 +5571,13 @@
       <c r="L89">
         <v>1</v>
       </c>
-      <c r="M89" s="8" t="s">
+      <c r="M89" s="7" t="s">
         <v>111</v>
       </c>
       <c r="N89">
         <v>0</v>
       </c>
-      <c r="O89" s="9">
+      <c r="O89" s="8">
         <v>0</v>
       </c>
       <c r="P89">
@@ -5596,7 +5597,7 @@
       <c r="C90">
         <v>13</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="25">
         <v>44026</v>
       </c>
       <c r="E90">
@@ -5620,13 +5621,13 @@
       <c r="L90">
         <v>1</v>
       </c>
-      <c r="M90" s="8" t="s">
+      <c r="M90" s="7" t="s">
         <v>112</v>
       </c>
       <c r="N90">
         <v>0</v>
       </c>
-      <c r="O90" s="9">
+      <c r="O90" s="8">
         <v>0</v>
       </c>
       <c r="P90">
@@ -5646,7 +5647,7 @@
       <c r="C91">
         <v>13</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D91" s="25">
         <v>44026</v>
       </c>
       <c r="E91">
@@ -5670,13 +5671,13 @@
       <c r="L91">
         <v>1</v>
       </c>
-      <c r="M91" s="8" t="s">
+      <c r="M91" s="7" t="s">
         <v>113</v>
       </c>
       <c r="N91">
         <v>0</v>
       </c>
-      <c r="O91" s="9">
+      <c r="O91" s="8">
         <v>0</v>
       </c>
       <c r="P91">
@@ -5696,7 +5697,7 @@
       <c r="C92">
         <v>13</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D92" s="25">
         <v>44026</v>
       </c>
       <c r="E92">
@@ -5723,13 +5724,13 @@
       <c r="L92">
         <v>1</v>
       </c>
-      <c r="M92" s="8" t="s">
+      <c r="M92" s="7" t="s">
         <v>114</v>
       </c>
       <c r="N92">
         <v>0</v>
       </c>
-      <c r="O92" s="9">
+      <c r="O92" s="8">
         <v>0</v>
       </c>
       <c r="P92">
@@ -5749,7 +5750,7 @@
       <c r="C93">
         <v>14</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D93" s="25">
         <v>44026</v>
       </c>
       <c r="E93">
@@ -5776,13 +5777,13 @@
       <c r="L93">
         <v>1</v>
       </c>
-      <c r="M93" s="8" t="s">
+      <c r="M93" s="7" t="s">
         <v>115</v>
       </c>
       <c r="N93">
         <v>0</v>
       </c>
-      <c r="O93" s="9">
+      <c r="O93" s="8">
         <v>0</v>
       </c>
       <c r="P93">
@@ -5802,7 +5803,7 @@
       <c r="C94">
         <v>14</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D94" s="25">
         <v>44026</v>
       </c>
       <c r="E94">
@@ -5829,13 +5830,13 @@
       <c r="L94">
         <v>1</v>
       </c>
-      <c r="M94" s="8" t="s">
+      <c r="M94" s="7" t="s">
         <v>116</v>
       </c>
       <c r="N94">
         <v>0</v>
       </c>
-      <c r="O94" s="9">
+      <c r="O94" s="8">
         <v>0</v>
       </c>
       <c r="P94">
@@ -5855,7 +5856,7 @@
       <c r="C95">
         <v>14</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D95" s="25">
         <v>44026</v>
       </c>
       <c r="E95">
@@ -5882,13 +5883,13 @@
       <c r="L95">
         <v>1</v>
       </c>
-      <c r="M95" s="8" t="s">
+      <c r="M95" s="7" t="s">
         <v>117</v>
       </c>
       <c r="N95">
         <v>0</v>
       </c>
-      <c r="O95" s="9">
+      <c r="O95" s="8">
         <v>0</v>
       </c>
       <c r="P95">
@@ -5908,7 +5909,7 @@
       <c r="C96">
         <v>6</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96" s="25">
         <v>44036</v>
       </c>
       <c r="E96">
@@ -5935,7 +5936,7 @@
       <c r="L96">
         <v>0</v>
       </c>
-      <c r="M96" s="7" t="s">
+      <c r="M96" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P96">
@@ -5955,7 +5956,7 @@
       <c r="C97">
         <v>6</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D97" s="25">
         <v>44036</v>
       </c>
       <c r="E97">
@@ -5982,7 +5983,7 @@
       <c r="L97">
         <v>0</v>
       </c>
-      <c r="M97" s="7" t="s">
+      <c r="M97" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P97">
@@ -6002,7 +6003,7 @@
       <c r="C98">
         <v>11</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D98" s="25">
         <v>44036</v>
       </c>
       <c r="E98">
@@ -6029,13 +6030,13 @@
       <c r="L98">
         <v>1</v>
       </c>
-      <c r="M98" s="8" t="s">
+      <c r="M98" s="7" t="s">
         <v>118</v>
       </c>
       <c r="N98">
         <v>0</v>
       </c>
-      <c r="O98" s="9">
+      <c r="O98" s="8">
         <v>0</v>
       </c>
       <c r="P98">
@@ -6055,7 +6056,7 @@
       <c r="C99">
         <v>11</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99" s="25">
         <v>44036</v>
       </c>
       <c r="E99">
@@ -6082,13 +6083,13 @@
       <c r="L99">
         <v>1</v>
       </c>
-      <c r="M99" s="8" t="s">
+      <c r="M99" s="7" t="s">
         <v>119</v>
       </c>
       <c r="N99">
         <v>0</v>
       </c>
-      <c r="O99" s="9">
+      <c r="O99" s="8">
         <v>0</v>
       </c>
       <c r="P99">
@@ -6108,7 +6109,7 @@
       <c r="C100">
         <v>6</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D100" s="25">
         <v>44036</v>
       </c>
       <c r="E100">
@@ -6135,7 +6136,7 @@
       <c r="L100">
         <v>0</v>
       </c>
-      <c r="M100" s="8"/>
+      <c r="M100" s="7"/>
       <c r="P100">
         <v>0</v>
       </c>
@@ -6153,7 +6154,7 @@
       <c r="C101">
         <v>6</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D101" s="25">
         <v>44036</v>
       </c>
       <c r="E101">
@@ -6180,7 +6181,7 @@
       <c r="L101">
         <v>0</v>
       </c>
-      <c r="M101" s="8"/>
+      <c r="M101" s="7"/>
       <c r="P101">
         <v>0</v>
       </c>
@@ -6198,7 +6199,7 @@
       <c r="C102">
         <v>8</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D102" s="25">
         <v>44036</v>
       </c>
       <c r="E102">
@@ -6225,7 +6226,7 @@
       <c r="L102">
         <v>1</v>
       </c>
-      <c r="M102" s="8" t="s">
+      <c r="M102" s="7" t="s">
         <v>120</v>
       </c>
       <c r="N102">
@@ -6251,7 +6252,7 @@
       <c r="C103">
         <v>6</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103" s="25">
         <v>44036</v>
       </c>
       <c r="E103">
@@ -6278,7 +6279,7 @@
       <c r="L103">
         <v>1</v>
       </c>
-      <c r="M103" s="8" t="s">
+      <c r="M103" s="7" t="s">
         <v>121</v>
       </c>
       <c r="N103">
@@ -6304,7 +6305,7 @@
       <c r="C104">
         <v>13</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104" s="25">
         <v>44036</v>
       </c>
       <c r="E104">
@@ -6331,13 +6332,13 @@
       <c r="L104">
         <v>1</v>
       </c>
-      <c r="M104" s="8" t="s">
+      <c r="M104" s="7" t="s">
         <v>122</v>
       </c>
       <c r="N104">
         <v>0</v>
       </c>
-      <c r="O104" s="9">
+      <c r="O104" s="8">
         <v>0</v>
       </c>
       <c r="P104">
@@ -6357,7 +6358,7 @@
       <c r="C105">
         <v>11</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105" s="25">
         <v>44036</v>
       </c>
       <c r="E105">
@@ -6384,13 +6385,13 @@
       <c r="L105">
         <v>1</v>
       </c>
-      <c r="M105" s="8" t="s">
+      <c r="M105" s="7" t="s">
         <v>123</v>
       </c>
       <c r="N105">
         <v>0</v>
       </c>
-      <c r="O105" s="9">
+      <c r="O105" s="8">
         <v>0</v>
       </c>
       <c r="P105">
@@ -6410,7 +6411,7 @@
       <c r="C106">
         <v>11</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106" s="25">
         <v>44036</v>
       </c>
       <c r="E106">
@@ -6437,13 +6438,13 @@
       <c r="L106">
         <v>1</v>
       </c>
-      <c r="M106" s="8" t="s">
+      <c r="M106" s="7" t="s">
         <v>124</v>
       </c>
       <c r="N106">
         <v>0</v>
       </c>
-      <c r="O106" s="9">
+      <c r="O106" s="8">
         <v>0</v>
       </c>
       <c r="P106">
@@ -6463,7 +6464,7 @@
       <c r="C107">
         <v>13</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107" s="25">
         <v>44036</v>
       </c>
       <c r="E107">
@@ -6490,13 +6491,13 @@
       <c r="L107">
         <v>1</v>
       </c>
-      <c r="M107" s="8" t="s">
+      <c r="M107" s="7" t="s">
         <v>125</v>
       </c>
       <c r="N107">
         <v>0</v>
       </c>
-      <c r="O107" s="9">
+      <c r="O107" s="8">
         <v>0</v>
       </c>
       <c r="P107">
@@ -6516,7 +6517,7 @@
       <c r="C108">
         <v>11</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108" s="25">
         <v>44036</v>
       </c>
       <c r="E108">
@@ -6543,13 +6544,13 @@
       <c r="L108">
         <v>1</v>
       </c>
-      <c r="M108" s="8" t="s">
+      <c r="M108" s="7" t="s">
         <v>126</v>
       </c>
       <c r="N108">
         <v>0</v>
       </c>
-      <c r="O108" s="9">
+      <c r="O108" s="8">
         <v>0</v>
       </c>
       <c r="P108">
@@ -6569,7 +6570,7 @@
       <c r="C109">
         <v>11</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109" s="25">
         <v>44036</v>
       </c>
       <c r="E109">
@@ -6596,13 +6597,13 @@
       <c r="L109">
         <v>1</v>
       </c>
-      <c r="M109" s="8" t="s">
+      <c r="M109" s="7" t="s">
         <v>127</v>
       </c>
       <c r="N109">
         <v>0</v>
       </c>
-      <c r="O109" s="9">
+      <c r="O109" s="8">
         <v>0</v>
       </c>
       <c r="P109">
@@ -6622,7 +6623,7 @@
       <c r="C110">
         <v>11</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110" s="25">
         <v>44036</v>
       </c>
       <c r="E110">
@@ -6649,13 +6650,13 @@
       <c r="L110">
         <v>1</v>
       </c>
-      <c r="M110" s="8" t="s">
+      <c r="M110" s="7" t="s">
         <v>128</v>
       </c>
       <c r="N110">
         <v>0</v>
       </c>
-      <c r="O110" s="9">
+      <c r="O110" s="8">
         <v>0</v>
       </c>
       <c r="P110">
@@ -6675,7 +6676,7 @@
       <c r="C111">
         <v>11</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111" s="25">
         <v>44036</v>
       </c>
       <c r="E111">
@@ -6702,13 +6703,13 @@
       <c r="L111">
         <v>1</v>
       </c>
-      <c r="M111" s="8" t="s">
+      <c r="M111" s="7" t="s">
         <v>129</v>
       </c>
       <c r="N111">
         <v>0</v>
       </c>
-      <c r="O111" s="9">
+      <c r="O111" s="8">
         <v>0</v>
       </c>
       <c r="P111">
@@ -6719,16 +6720,16 @@
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A112" s="11">
+      <c r="A112" s="10">
         <v>113</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="B112" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C112">
         <v>52</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D112" s="25" t="s">
         <v>130</v>
       </c>
       <c r="E112">
@@ -6755,11 +6756,11 @@
       <c r="L112">
         <v>1</v>
       </c>
-      <c r="M112" s="8"/>
-      <c r="N112" s="10">
-        <v>1</v>
-      </c>
-      <c r="O112" s="10">
+      <c r="M112" s="7"/>
+      <c r="N112" s="9">
+        <v>1</v>
+      </c>
+      <c r="O112" s="9">
         <v>512</v>
       </c>
       <c r="P112">
@@ -6773,16 +6774,16 @@
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A113" s="11">
+      <c r="A113" s="10">
         <v>114</v>
       </c>
-      <c r="B113" s="11" t="s">
+      <c r="B113" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C113">
         <v>52</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D113" s="25" t="s">
         <v>130</v>
       </c>
       <c r="E113">
@@ -6806,14 +6807,14 @@
       <c r="K113">
         <v>1</v>
       </c>
-      <c r="L113" s="10">
-        <v>1</v>
-      </c>
-      <c r="M113" s="8"/>
-      <c r="N113" s="10">
-        <v>1</v>
-      </c>
-      <c r="O113" s="10">
+      <c r="L113" s="9">
+        <v>1</v>
+      </c>
+      <c r="M113" s="7"/>
+      <c r="N113" s="9">
+        <v>1</v>
+      </c>
+      <c r="O113" s="9">
         <v>512</v>
       </c>
       <c r="P113">
@@ -6824,16 +6825,16 @@
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A114" s="11">
+      <c r="A114" s="10">
         <v>115</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C114">
         <v>52</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="25">
         <v>44090</v>
       </c>
       <c r="E114">
@@ -6860,7 +6861,7 @@
       <c r="L114">
         <v>0</v>
       </c>
-      <c r="M114" s="8"/>
+      <c r="M114" s="7"/>
       <c r="P114">
         <v>0</v>
       </c>
@@ -6879,7 +6880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC7E540-CE28-4BDB-BE4A-3ACAD08B4B6E}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
@@ -6887,230 +6888,230 @@
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="142.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="24" t="s">
+    <row r="1" spans="1:6" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="19">
         <v>43990</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>43945</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>43989</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <v>43945</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>43988</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>43958</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>43954</v>
       </c>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>43958</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>43989</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>43982</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+    <row r="7" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>43989</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>43982</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>43990</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>43984</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="15">
         <v>43980</v>
       </c>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>43992</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>43990</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <v>43997</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>43996</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>43990</v>
       </c>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="19">
         <v>43997</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>43996</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>43989</v>
       </c>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="19">
         <v>44090</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>44089</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>44086</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="9"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="9"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="9"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="9"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="9"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="9"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="9"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="9"/>
+      <c r="E21" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7127,414 +7128,414 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>8</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>8</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>8</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>8</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>8</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>8</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>8</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>8</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>8</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>18</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>8</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>8</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>8</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>8</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>8</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>8</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5" t="s">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4" t="s">
         <v>105</v>
       </c>
     </row>
@@ -7768,18 +7769,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7802,18 +7803,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DE64F8C-143D-48F5-BA11-F9621BE3BA9D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA11E8EA-6BCB-4153-9E3A-290799CFE621}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DE64F8C-143D-48F5-BA11-F9621BE3BA9D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>